<commit_message>
refactor 4: CMM045: Update chuc nang in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/CMM045_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/CMM045_template.xlsx
@@ -133,7 +133,6 @@
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">承認一覧!$A$1:$J$66</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">承認一覧!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">申請一覧!$1:$2</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[9]!PrintDaicho</definedName>
@@ -267,7 +266,7 @@
     <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
     <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -283,10 +282,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>　</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;=dataSource.applicantName</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.appType</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.prePostAtr</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.appStartDate</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.appContent</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.inputDate</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.reflectionStatus</t>
+  </si>
+  <si>
+    <t>&amp;=dataSource.approvalStatusInquiry</t>
   </si>
 </sst>
 </file>
@@ -44470,14 +44493,30 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="2:10" ht="20.25" customHeight="1">
       <c r="B4" s="4"/>
@@ -44553,14 +44592,30 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="2:10" ht="20.25" customHeight="1">
       <c r="B4" s="4"/>

</xml_diff>

<commit_message>
refactor 4: CMM045: Update UI
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/CMM045_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/CMM045_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Project\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\C_共通\CMM_申請承認一覧\CMM045_申請一覧・承認一覧\ver4~\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9AC928-695E-43A6-A954-9E7D2E1CEF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="510" windowWidth="20250" windowHeight="13620"/>
+    <workbookView xWindow="3390" yWindow="510" windowWidth="20250" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="承認一覧" sheetId="29" r:id="rId1"/>
@@ -32,6 +33,7 @@
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
@@ -55,7 +57,7 @@
     <definedName name="_Sort" hidden="1">#REF!</definedName>
     <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
-    <definedName name="a">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a">'[2]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
     <definedName name="AAAA" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="AAAA" localSheetId="1" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
@@ -73,24 +75,24 @@
     <definedName name="ｂｂｂｂ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｂｂｂｂ" localSheetId="1" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｂｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="cal_index_size" localSheetId="0">[2]!cal_index_size</definedName>
-    <definedName name="cal_index_size" localSheetId="1">[2]!cal_index_size</definedName>
-    <definedName name="cal_index_size">[2]!cal_index_size</definedName>
-    <definedName name="cal_table_size" localSheetId="0">[2]!cal_table_size</definedName>
-    <definedName name="cal_table_size" localSheetId="1">[2]!cal_table_size</definedName>
-    <definedName name="cal_table_size">[2]!cal_table_size</definedName>
+    <definedName name="cal_index_size" localSheetId="0">[3]!cal_index_size</definedName>
+    <definedName name="cal_index_size" localSheetId="1">[3]!cal_index_size</definedName>
+    <definedName name="cal_index_size">[3]!cal_index_size</definedName>
+    <definedName name="cal_table_size" localSheetId="0">[3]!cal_table_size</definedName>
+    <definedName name="cal_table_size" localSheetId="1">[3]!cal_table_size</definedName>
+    <definedName name="cal_table_size">[3]!cal_table_size</definedName>
     <definedName name="ccc" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ccc" localSheetId="1" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ccc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ｃｃｃｃ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｃｃｃｃ" localSheetId="1" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｃｃｃｃ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
-    <definedName name="CULC.cal_index_size" localSheetId="0">[3]!CULC.cal_index_size</definedName>
-    <definedName name="CULC.cal_index_size" localSheetId="1">[3]!CULC.cal_index_size</definedName>
-    <definedName name="CULC.cal_index_size">[3]!CULC.cal_index_size</definedName>
-    <definedName name="C保守委託単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守支援単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="CULC.cal_index_size" localSheetId="0">[4]!CULC.cal_index_size</definedName>
+    <definedName name="CULC.cal_index_size" localSheetId="1">[4]!CULC.cal_index_size</definedName>
+    <definedName name="CULC.cal_index_size">[4]!CULC.cal_index_size</definedName>
+    <definedName name="C保守委託単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守支援単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価">'[5]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="DDDD" localSheetId="1" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
@@ -101,7 +103,7 @@
     <definedName name="e" localSheetId="1" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｈｈｈ">#REF!</definedName>
-    <definedName name="HW9707K">[5]仕切価格!$B$1:$BD$231</definedName>
+    <definedName name="HW9707K">[6]仕切価格!$B$1:$BD$231</definedName>
     <definedName name="ＩＨ">#REF!</definedName>
     <definedName name="item1">#REF!</definedName>
     <definedName name="Ｉホ">#REF!</definedName>
@@ -122,26 +124,26 @@
     <definedName name="Ｌホ">#REF!</definedName>
     <definedName name="ＭＨ">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
-    <definedName name="ｎ">'[6]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ">'[7]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="ＯＨ">#REF!</definedName>
-    <definedName name="OPT_NO" localSheetId="0">[7]!OPT_NO</definedName>
-    <definedName name="OPT_NO" localSheetId="1">[7]!OPT_NO</definedName>
-    <definedName name="OPT_NO">[7]!OPT_NO</definedName>
-    <definedName name="OPT_YES" localSheetId="0">[7]!OPT_YES</definedName>
-    <definedName name="OPT_YES" localSheetId="1">[7]!OPT_YES</definedName>
-    <definedName name="OPT_YES">[7]!OPT_YES</definedName>
+    <definedName name="OPT_NO" localSheetId="0">[8]!OPT_NO</definedName>
+    <definedName name="OPT_NO" localSheetId="1">[8]!OPT_NO</definedName>
+    <definedName name="OPT_NO">[8]!OPT_NO</definedName>
+    <definedName name="OPT_YES" localSheetId="0">[8]!OPT_YES</definedName>
+    <definedName name="OPT_YES" localSheetId="1">[8]!OPT_YES</definedName>
+    <definedName name="OPT_YES">[8]!OPT_YES</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
-    <definedName name="PG単価">[8]明細合計!#REF!</definedName>
+    <definedName name="PG単価">[9]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">承認一覧!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">申請一覧!$1:$2</definedName>
-    <definedName name="PrintDaicho" localSheetId="0">[9]!PrintDaicho</definedName>
-    <definedName name="PrintDaicho" localSheetId="1">[9]!PrintDaicho</definedName>
-    <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
-    <definedName name="QuitDaicho" localSheetId="0">[9]!QuitDaicho</definedName>
-    <definedName name="QuitDaicho" localSheetId="1">[9]!QuitDaicho</definedName>
-    <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
-    <definedName name="SE単価">[8]明細合計!#REF!</definedName>
+    <definedName name="PrintDaicho" localSheetId="0">[10]!PrintDaicho</definedName>
+    <definedName name="PrintDaicho" localSheetId="1">[10]!PrintDaicho</definedName>
+    <definedName name="PrintDaicho">[10]!PrintDaicho</definedName>
+    <definedName name="QuitDaicho" localSheetId="0">[10]!QuitDaicho</definedName>
+    <definedName name="QuitDaicho" localSheetId="1">[10]!QuitDaicho</definedName>
+    <definedName name="QuitDaicho">[10]!QuitDaicho</definedName>
+    <definedName name="SE単価">[9]明細合計!#REF!</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
@@ -151,8 +153,8 @@
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" hidden="1">#REF!</definedName>
-    <definedName name="ｗ">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="WC単価">'[4]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
+    <definedName name="ｗ">'[5]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="WC単価">'[5]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
     <definedName name="wrn.MIND." localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.MIND." localSheetId="1" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.MIND." hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -177,11 +179,11 @@
     <definedName name="クにＨ">#REF!</definedName>
     <definedName name="クニホ">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
-    <definedName name="サＨ">'[10]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ">'[10]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ">'[11]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サホ">'[11]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
     <definedName name="サホ1">#REF!</definedName>
     <definedName name="ツール別見積工数">#REF!</definedName>
-    <definedName name="テーブル項目">[11]項目定義書!$A$3:$E$364</definedName>
+    <definedName name="テーブル項目">[12]項目定義書!$A$3:$E$364</definedName>
     <definedName name="ハ１">#REF!</definedName>
     <definedName name="は２">#REF!</definedName>
     <definedName name="ハ２ホ">#REF!</definedName>
@@ -192,14 +194,14 @@
     <definedName name="ハホ">#REF!</definedName>
     <definedName name="ファイル展開">#N/A</definedName>
     <definedName name="ヘッダー">#REF!</definedName>
-    <definedName name="ユーザー一覧">'[12]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
-    <definedName name="ワイドに" localSheetId="0">[13]!ワイドに</definedName>
-    <definedName name="ワイドに" localSheetId="1">[13]!ワイドに</definedName>
-    <definedName name="ワイドに">[13]!ワイドに</definedName>
+    <definedName name="ユーザー一覧">'[13]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
+    <definedName name="ワイドに" localSheetId="0">[14]!ワイドに</definedName>
+    <definedName name="ワイドに" localSheetId="1">[14]!ワイドに</definedName>
+    <definedName name="ワイドに">[14]!ワイドに</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
-    <definedName name="印刷" localSheetId="0">[14]!印刷</definedName>
-    <definedName name="印刷" localSheetId="1">[14]!印刷</definedName>
-    <definedName name="印刷">[14]!印刷</definedName>
+    <definedName name="印刷" localSheetId="0">[15]!印刷</definedName>
+    <definedName name="印刷" localSheetId="1">[15]!印刷</definedName>
+    <definedName name="印刷">[15]!印刷</definedName>
     <definedName name="価格表">#REF!</definedName>
     <definedName name="画面1">#REF!</definedName>
     <definedName name="画面2">#REF!</definedName>
@@ -215,14 +217,14 @@
     <definedName name="関連表" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
-    <definedName name="機種SORT">[15]!機種SORT</definedName>
+    <definedName name="機種SORT">[16]!機種SORT</definedName>
     <definedName name="機能別原価">#REF!</definedName>
     <definedName name="銀行の登録48">#REF!</definedName>
     <definedName name="銀行の登録67">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
-    <definedName name="見やすく" localSheetId="0">[13]!見やすく</definedName>
-    <definedName name="見やすく" localSheetId="1">[13]!見やすく</definedName>
-    <definedName name="見やすく">[13]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="0">[14]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="1">[14]!見やすく</definedName>
+    <definedName name="見やすく">[14]!見やすく</definedName>
     <definedName name="見積工数">#REF!</definedName>
     <definedName name="原価">#REF!</definedName>
     <definedName name="工程別生産性">#REF!</definedName>
@@ -234,13 +236,13 @@
     <definedName name="項目名の登録6">#REF!</definedName>
     <definedName name="項目名の登録7">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
-    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="仕切り">'[5]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[5]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="社共単価">'[5]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
     <definedName name="種別">#REF!</definedName>
-    <definedName name="終了" localSheetId="0">[16]!終了</definedName>
-    <definedName name="終了" localSheetId="1">[16]!終了</definedName>
-    <definedName name="終了">[16]!終了</definedName>
+    <definedName name="終了" localSheetId="0">[17]!終了</definedName>
+    <definedName name="終了" localSheetId="1">[17]!終了</definedName>
+    <definedName name="終了">[17]!終了</definedName>
     <definedName name="住民税115">#REF!</definedName>
     <definedName name="住民税96">#REF!</definedName>
     <definedName name="住民税納付先の登録7">#REF!</definedName>
@@ -250,23 +252,23 @@
     <definedName name="設計書">#N/A</definedName>
     <definedName name="単価">#REF!</definedName>
     <definedName name="単価種別">#REF!</definedName>
-    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="値引単価">'[5]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="直扱単価">'[5]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
     <definedName name="定価">#REF!</definedName>
     <definedName name="電車">#REF!</definedName>
     <definedName name="日帰り">#REF!</definedName>
     <definedName name="日帰り単金">#REF!</definedName>
     <definedName name="売値">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
-    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
-    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="備考">'[5]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="標準価格">'[5]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="部">'[5]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
     <definedName name="部門別時間外労働手当状況">#REF!</definedName>
-    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
+    <definedName name="保守委託単価">'[5]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[5]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="保守単価">'[5]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -282,45 +284,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>　</t>
     <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=dataSource.applicantName</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.appType</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.prePostAtr</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.appStartDate</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.appContent</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.inputDate</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.reflectionStatus</t>
-  </si>
-  <si>
-    <t>&amp;=dataSource.approvalStatusInquiry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -328,14 +306,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -356,7 +334,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -438,6 +416,9 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -455,18 +436,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2"/>
-    <cellStyle name="標準 2" xfId="1"/>
-    <cellStyle name="標準 2 2" xfId="4"/>
-    <cellStyle name="標準 3" xfId="3"/>
-    <cellStyle name="標準 3 2 2" xfId="5"/>
-    <cellStyle name="標準 4" xfId="6"/>
+    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準 4" xfId="6" xr:uid="{3D1351D6-C7CC-43D0-8B9C-37BA0A2C7DCA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -491,20 +469,57 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
-      <sheetName val="master"/>
-      <sheetName val="Sheet1"/>
+      <sheetName val="表紙"/>
+      <sheetName val="目次"/>
+      <sheetName val="修正履歴"/>
+      <sheetName val="帳票イメージ"/>
+      <sheetName val="帳票レイアウト"/>
+      <sheetName val="項目定義"/>
+      <sheetName val="項目制御"/>
+      <sheetName val="項目移送表"/>
+      <sheetName val="多言語参照"/>
+      <sheetName val="補足資料"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="収印ﾓﾆﾀｰ"/>
+      <sheetName val="収印ﾓﾆﾀｰ.XLS"/>
+      <sheetName val="%E5%8F%8E%E5%8D%B0%EF%BE%93%EF%"/>
+      <sheetName val="JOB一覧表"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="PrintDaicho"/>
+      <definedName name="QuitDaicho"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -517,7 +532,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -5813,7 +5828,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -5846,7 +5861,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -5995,7 +6010,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6011,7 +6026,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6029,7 +6044,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6046,6 +6061,23 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="master"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6068,7 +6100,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6150,7 +6182,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -7634,7 +7666,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -43996,7 +44028,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44009,7 +44041,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44028,7 +44060,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -44036,29 +44068,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="収印ﾓﾆﾀｰ"/>
-      <sheetName val="収印ﾓﾆﾀｰ.XLS"/>
-      <sheetName val="%E5%8F%8E%E5%8D%B0%EF%BE%93%EF%"/>
-      <sheetName val="JOB一覧表"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="PrintDaicho"/>
-      <definedName name="QuitDaicho"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44449,90 +44458,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEFE533-6CC0-4C9B-88F8-BA3085EB50C4}">
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="0.75" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="0.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="0.77734375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" customHeight="1">
+    <row r="1" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="2" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>8</v>
-      </c>
+    <row r="3" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+    <row r="4" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:10" ht="12" customHeight="1"/>
-    <row r="6" spans="2:10" ht="12" customHeight="1"/>
-    <row r="7" spans="2:10" ht="12" customHeight="1"/>
-    <row r="8" spans="2:10" ht="12" customHeight="1"/>
-    <row r="9" spans="2:10" ht="12" customHeight="1"/>
+    <row r="5" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:I1"/>
@@ -44548,90 +44541,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F84D19-41C4-4404-A90D-BA4A44465E16}">
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="0.75" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="0.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="0.77734375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" customHeight="1">
+    <row r="1" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="2" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>8</v>
-      </c>
+    <row r="3" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="2:10" ht="20.25" customHeight="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+    <row r="4" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:10" ht="12" customHeight="1"/>
-    <row r="6" spans="2:10" ht="12" customHeight="1"/>
-    <row r="7" spans="2:10" ht="12" customHeight="1"/>
-    <row r="8" spans="2:10" ht="12" customHeight="1"/>
-    <row r="9" spans="2:10" ht="12" customHeight="1"/>
+    <row r="5" spans="2:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:I1"/>

</xml_diff>